<commit_message>
Validation Code in place before population
</commit_message>
<xml_diff>
--- a/group1/datasets/dit group project - sample dataset.xlsx
+++ b/group1/datasets/dit group project - sample dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Base Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2393" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="341">
   <si>
     <t>Date / Time</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>12A</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
   <si>
     <t>Description</t>
@@ -1167,10 +1170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1003"/>
+  <dimension ref="A1:N1013"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A993" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C1003" activeCellId="0" pane="topLeft" sqref="C1003"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A768" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C1013" activeCellId="0" pane="topLeft" sqref="C1013"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -45320,6 +45323,11 @@
       </c>
       <c r="N1003" s="2" t="n">
         <v>1.15044494090948E+018</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1013">
+      <c r="C1013" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -45363,7 +45371,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -45374,7 +45382,7 @@
         <v>4097</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
@@ -45385,7 +45393,7 @@
         <v>4097</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
@@ -45396,7 +45404,7 @@
         <v>4097</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
@@ -45407,7 +45415,7 @@
         <v>4097</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
@@ -45418,7 +45426,7 @@
         <v>4097</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
@@ -45429,7 +45437,7 @@
         <v>4097</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
@@ -45440,7 +45448,7 @@
         <v>4097</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
@@ -45451,7 +45459,7 @@
         <v>4097</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
@@ -45462,7 +45470,7 @@
         <v>4097</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
@@ -45473,7 +45481,7 @@
         <v>4097</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
@@ -45484,7 +45492,7 @@
         <v>4097</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
@@ -45495,7 +45503,7 @@
         <v>4097</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
@@ -45506,7 +45514,7 @@
         <v>4097</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
@@ -45517,7 +45525,7 @@
         <v>4097</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
@@ -45528,7 +45536,7 @@
         <v>4097</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
@@ -45539,7 +45547,7 @@
         <v>4097</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
@@ -45550,7 +45558,7 @@
         <v>4097</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
@@ -45561,7 +45569,7 @@
         <v>4098</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
@@ -45572,7 +45580,7 @@
         <v>4098</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
@@ -45583,7 +45591,7 @@
         <v>4098</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
@@ -45594,7 +45602,7 @@
         <v>4098</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
@@ -45605,7 +45613,7 @@
         <v>4125</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
@@ -45616,7 +45624,7 @@
         <v>4125</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
@@ -45627,7 +45635,7 @@
         <v>4125</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
@@ -45638,7 +45646,7 @@
         <v>4125</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
@@ -45649,7 +45657,7 @@
         <v>4125</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
@@ -45660,7 +45668,7 @@
         <v>4125</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
@@ -45671,7 +45679,7 @@
         <v>4125</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
@@ -45682,7 +45690,7 @@
         <v>4125</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
@@ -45693,7 +45701,7 @@
         <v>4125</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
@@ -45704,7 +45712,7 @@
         <v>4125</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
@@ -45715,7 +45723,7 @@
         <v>4125</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
@@ -45726,7 +45734,7 @@
         <v>4125</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
@@ -45737,7 +45745,7 @@
         <v>4125</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
@@ -45748,7 +45756,7 @@
         <v>4125</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
@@ -45759,7 +45767,7 @@
         <v>4125</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
@@ -45770,7 +45778,7 @@
         <v>4125</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
@@ -45781,7 +45789,7 @@
         <v>4125</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
@@ -45792,7 +45800,7 @@
         <v>4125</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
@@ -45803,7 +45811,7 @@
         <v>4125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
@@ -45814,7 +45822,7 @@
         <v>4125</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
@@ -45825,7 +45833,7 @@
         <v>4125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
@@ -45836,7 +45844,7 @@
         <v>4125</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
@@ -45847,7 +45855,7 @@
         <v>4125</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
@@ -45858,7 +45866,7 @@
         <v>4125</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
@@ -45869,7 +45877,7 @@
         <v>4125</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
@@ -45880,7 +45888,7 @@
         <v>4125</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
@@ -45891,7 +45899,7 @@
         <v>4125</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
@@ -45902,7 +45910,7 @@
         <v>4125</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
@@ -45913,7 +45921,7 @@
         <v>4125</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
@@ -45924,7 +45932,7 @@
         <v>4125</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="53">
@@ -45935,7 +45943,7 @@
         <v>4125</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="54">
@@ -45946,7 +45954,7 @@
         <v>4125</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
@@ -45957,7 +45965,7 @@
         <v>4125</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
@@ -45968,7 +45976,7 @@
         <v>4125</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="57">
@@ -45979,7 +45987,7 @@
         <v>4106</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
@@ -45990,7 +45998,7 @@
         <v>4106</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="59">
@@ -46001,7 +46009,7 @@
         <v>4106</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="60">
@@ -46012,7 +46020,7 @@
         <v>4106</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="61">
@@ -46023,7 +46031,7 @@
         <v>4106</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
@@ -46034,7 +46042,7 @@
         <v>4106</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
@@ -46045,7 +46053,7 @@
         <v>4106</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="64">
@@ -46056,7 +46064,7 @@
         <v>4106</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="65">
@@ -46067,7 +46075,7 @@
         <v>4106</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="66">
@@ -46078,7 +46086,7 @@
         <v>4106</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="67">
@@ -46089,7 +46097,7 @@
         <v>4106</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
@@ -46100,7 +46108,7 @@
         <v>4106</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="69">
@@ -46111,7 +46119,7 @@
         <v>4106</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
@@ -46122,7 +46130,7 @@
         <v>4106</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
@@ -46133,7 +46141,7 @@
         <v>4106</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="72">
@@ -46144,7 +46152,7 @@
         <v>4106</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="73">
@@ -46155,7 +46163,7 @@
         <v>4106</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="74">
@@ -46166,7 +46174,7 @@
         <v>4106</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="75">
@@ -46177,7 +46185,7 @@
         <v>4106</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="76">
@@ -46188,7 +46196,7 @@
         <v>4106</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="77">
@@ -46199,7 +46207,7 @@
         <v>4106</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="78">
@@ -46210,7 +46218,7 @@
         <v>4106</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="79">
@@ -46221,7 +46229,7 @@
         <v>4106</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="80">
@@ -46232,7 +46240,7 @@
         <v>4106</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="81">
@@ -46243,7 +46251,7 @@
         <v>4106</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -46266,8 +46274,8 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -46283,7 +46291,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -46291,15 +46299,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
@@ -46307,7 +46313,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
@@ -46315,15 +46321,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -46365,31 +46369,31 @@
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="1" s="6">
       <c r="A1" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -46397,19 +46401,19 @@
         <v>100100</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>15</v>
@@ -46426,28 +46430,28 @@
         <v>100200</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>116</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
@@ -46455,22 +46459,22 @@
         <v>100300</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>120</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>15</v>
@@ -46484,19 +46488,19 @@
         <v>100400</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>122</v>
-      </c>
       <c r="F5" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>15</v>
@@ -46513,22 +46517,22 @@
         <v>100500</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>124</v>
-      </c>
       <c r="F6" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>15</v>
@@ -46542,19 +46546,19 @@
         <v>100600</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>127</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>15</v>
@@ -46571,19 +46575,19 @@
         <v>100700</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>130</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>15</v>
@@ -46600,19 +46604,19 @@
         <v>100800</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>132</v>
-      </c>
       <c r="F9" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>15</v>
@@ -46629,19 +46633,19 @@
         <v>100900</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>15</v>
@@ -46658,19 +46662,19 @@
         <v>101000</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>15</v>
@@ -46687,19 +46691,19 @@
         <v>101300</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>136</v>
-      </c>
       <c r="F12" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>15</v>
@@ -46716,22 +46720,22 @@
         <v>101500</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>139</v>
-      </c>
       <c r="G13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>15</v>
@@ -46745,19 +46749,19 @@
         <v>101600</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>141</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>15</v>
@@ -46774,22 +46778,22 @@
         <v>101700</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>144</v>
-      </c>
       <c r="G15" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>15</v>
@@ -46803,22 +46807,22 @@
         <v>101710</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>146</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>15</v>
@@ -46832,22 +46836,22 @@
         <v>101800</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>149</v>
-      </c>
       <c r="G17" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>15</v>
@@ -46861,28 +46865,28 @@
         <v>102000</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>152</v>
-      </c>
       <c r="F18" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
@@ -46890,19 +46894,19 @@
         <v>102100</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>156</v>
-      </c>
       <c r="F19" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>15</v>
@@ -46919,19 +46923,19 @@
         <v>102200</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="F20" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>15</v>
@@ -46948,22 +46952,22 @@
         <v>102300</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>160</v>
-      </c>
       <c r="F21" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H21" s="0" t="s">
         <v>15</v>
@@ -46977,19 +46981,19 @@
         <v>102400</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>162</v>
-      </c>
       <c r="F22" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>15</v>
@@ -47006,19 +47010,19 @@
         <v>102500</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>164</v>
-      </c>
       <c r="F23" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>15</v>
@@ -47035,19 +47039,19 @@
         <v>102600</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>166</v>
-      </c>
       <c r="F24" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>15</v>
@@ -47064,22 +47068,22 @@
         <v>102700</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>169</v>
-      </c>
       <c r="G25" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>15</v>
@@ -47093,19 +47097,19 @@
         <v>102800</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>171</v>
-      </c>
       <c r="F26" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>15</v>
@@ -47122,19 +47126,19 @@
         <v>102900</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>173</v>
-      </c>
       <c r="F27" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>15</v>
@@ -47151,19 +47155,19 @@
         <v>103000</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>175</v>
-      </c>
       <c r="F28" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>15</v>
@@ -47180,19 +47184,19 @@
         <v>103100</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>177</v>
-      </c>
       <c r="F29" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>15</v>
@@ -47209,19 +47213,19 @@
         <v>103200</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C30" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>179</v>
-      </c>
       <c r="F30" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>15</v>
@@ -47238,19 +47242,19 @@
         <v>103300</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C31" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="F31" s="0" t="s">
         <v>183</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>182</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>15</v>
@@ -47267,22 +47271,22 @@
         <v>103500</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>184</v>
-      </c>
       <c r="F32" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>15</v>
@@ -47296,22 +47300,22 @@
         <v>103600</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="F33" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>187</v>
-      </c>
       <c r="G33" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>15</v>
@@ -47325,19 +47329,19 @@
         <v>103700</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>189</v>
-      </c>
       <c r="F34" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>15</v>
@@ -47354,19 +47358,19 @@
         <v>103800</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>191</v>
-      </c>
       <c r="F35" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>15</v>
@@ -47383,19 +47387,19 @@
         <v>103900</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C36" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>193</v>
-      </c>
       <c r="F36" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>15</v>
@@ -47412,19 +47416,19 @@
         <v>104100</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C37" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>195</v>
-      </c>
       <c r="F37" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>15</v>
@@ -47441,19 +47445,19 @@
         <v>104200</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C38" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>197</v>
-      </c>
       <c r="F38" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>15</v>
@@ -47470,19 +47474,19 @@
         <v>104400</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C39" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>199</v>
-      </c>
       <c r="F39" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>15</v>
@@ -47499,19 +47503,19 @@
         <v>104500</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C40" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>201</v>
-      </c>
       <c r="F40" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>15</v>
@@ -47528,19 +47532,19 @@
         <v>104600</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C41" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>203</v>
-      </c>
       <c r="F41" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>15</v>
@@ -47557,19 +47561,19 @@
         <v>104700</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C42" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>205</v>
-      </c>
       <c r="F42" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>15</v>
@@ -47586,19 +47590,19 @@
         <v>104800</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C43" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>207</v>
-      </c>
       <c r="F43" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G43" s="0" t="s">
         <v>15</v>
@@ -47615,19 +47619,19 @@
         <v>105000</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C44" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>209</v>
-      </c>
       <c r="F44" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G44" s="0" t="s">
         <v>15</v>
@@ -47644,19 +47648,19 @@
         <v>105200</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C45" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>211</v>
-      </c>
       <c r="F45" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G45" s="0" t="s">
         <v>15</v>
@@ -47673,22 +47677,22 @@
         <v>105300</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C46" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>213</v>
-      </c>
       <c r="F46" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H46" s="0" t="s">
         <v>15</v>
@@ -47702,19 +47706,19 @@
         <v>105400</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C47" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>215</v>
-      </c>
       <c r="F47" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>15</v>
@@ -47731,19 +47735,19 @@
         <v>105500</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C48" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>217</v>
-      </c>
       <c r="F48" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>15</v>
@@ -47760,19 +47764,19 @@
         <v>105600</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C49" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>219</v>
-      </c>
       <c r="F49" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G49" s="0" t="s">
         <v>15</v>
@@ -47789,19 +47793,19 @@
         <v>105700</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C50" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E50" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>221</v>
-      </c>
       <c r="F50" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>15</v>
@@ -47818,19 +47822,19 @@
         <v>105900</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C51" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E51" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>223</v>
-      </c>
       <c r="F51" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>15</v>
@@ -47847,22 +47851,22 @@
         <v>106200</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C52" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>225</v>
-      </c>
       <c r="F52" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H52" s="0" t="s">
         <v>15</v>
@@ -47876,19 +47880,19 @@
         <v>106400</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C53" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="D53" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>227</v>
-      </c>
       <c r="F53" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>15</v>
@@ -47905,19 +47909,19 @@
         <v>106500</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C54" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>229</v>
-      </c>
       <c r="F54" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>15</v>
@@ -47934,19 +47938,19 @@
         <v>106600</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C55" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E55" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>231</v>
-      </c>
       <c r="F55" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>15</v>
@@ -47963,19 +47967,19 @@
         <v>106700</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C56" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="D56" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>233</v>
-      </c>
       <c r="F56" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G56" s="0" t="s">
         <v>15</v>
@@ -47992,19 +47996,19 @@
         <v>106900</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C57" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>235</v>
-      </c>
       <c r="F57" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G57" s="0" t="s">
         <v>15</v>
@@ -48021,19 +48025,19 @@
         <v>107100</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C58" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E58" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>237</v>
-      </c>
       <c r="F58" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>15</v>
@@ -48050,28 +48054,28 @@
         <v>107200</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="60">
@@ -48079,19 +48083,19 @@
         <v>107400</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C60" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E60" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>242</v>
-      </c>
       <c r="F60" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G60" s="0" t="s">
         <v>15</v>
@@ -48108,19 +48112,19 @@
         <v>107600</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C61" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>244</v>
-      </c>
       <c r="F61" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>15</v>
@@ -48137,19 +48141,19 @@
         <v>107700</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C62" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="E62" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="F62" s="0" t="s">
         <v>248</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>247</v>
       </c>
       <c r="G62" s="0" t="s">
         <v>15</v>
@@ -48169,16 +48173,16 @@
         <v>247910</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>247910</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G63" s="0" t="s">
         <v>15</v>
@@ -48195,19 +48199,19 @@
         <v>107900</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C64" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E64" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>250</v>
-      </c>
       <c r="F64" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G64" s="0" t="s">
         <v>15</v>
@@ -48224,19 +48228,19 @@
         <v>108000</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C65" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E65" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>252</v>
-      </c>
       <c r="F65" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G65" s="0" t="s">
         <v>15</v>
@@ -48253,19 +48257,19 @@
         <v>108100</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C66" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="E66" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="F66" s="0" t="s">
         <v>256</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>255</v>
       </c>
       <c r="G66" s="0" t="s">
         <v>15</v>
@@ -48282,19 +48286,19 @@
         <v>108200</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C67" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E67" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>257</v>
-      </c>
       <c r="F67" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G67" s="0" t="s">
         <v>15</v>
@@ -48311,19 +48315,19 @@
         <v>108300</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C68" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E68" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="D68" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>259</v>
-      </c>
       <c r="F68" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>15</v>
@@ -48340,22 +48344,22 @@
         <v>108400</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C69" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="E69" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="F69" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E69" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>262</v>
-      </c>
       <c r="G69" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H69" s="0" t="s">
         <v>15</v>
@@ -48369,19 +48373,19 @@
         <v>116000</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>15</v>
@@ -48398,19 +48402,19 @@
         <v>21060800</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C71" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="D71" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>265</v>
-      </c>
       <c r="F71" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>15</v>
@@ -48427,19 +48431,19 @@
         <v>33000153</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C72" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E72" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="F72" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="F72" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>15</v>
@@ -48456,19 +48460,19 @@
         <v>33000253</v>
       </c>
       <c r="B73" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D73" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="C73" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="D73" s="0" t="s">
+      <c r="E73" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="F73" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="F73" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G73" s="0" t="s">
         <v>15</v>
@@ -48485,19 +48489,19 @@
         <v>33000353</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C74" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E74" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="D74" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>271</v>
-      </c>
       <c r="F74" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G74" s="0" t="s">
         <v>15</v>
@@ -48514,19 +48518,19 @@
         <v>33000453</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D75" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F75" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="F75" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G75" s="0" t="s">
         <v>15</v>
@@ -48543,19 +48547,19 @@
         <v>33000553</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D76" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="F76" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="F76" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G76" s="0" t="s">
         <v>15</v>
@@ -48572,19 +48576,19 @@
         <v>33000635</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C77" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E77" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="D77" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>275</v>
-      </c>
       <c r="F77" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G77" s="0" t="s">
         <v>15</v>
@@ -48601,19 +48605,19 @@
         <v>33000753</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D78" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="F78" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="F78" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G78" s="0" t="s">
         <v>15</v>
@@ -48630,19 +48634,19 @@
         <v>33000853</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D79" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="F79" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="F79" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G79" s="0" t="s">
         <v>15</v>
@@ -48659,19 +48663,19 @@
         <v>33000953</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D80" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="F80" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G80" s="0" t="s">
         <v>15</v>
@@ -48688,19 +48692,19 @@
         <v>33001053</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D81" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="F81" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E81" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="F81" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G81" s="0" t="s">
         <v>15</v>
@@ -48717,19 +48721,19 @@
         <v>33001195</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G82" s="0" t="s">
         <v>15</v>
@@ -48746,19 +48750,19 @@
         <v>33001235</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G83" s="0" t="s">
         <v>15</v>
@@ -48775,19 +48779,19 @@
         <v>33001295</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G84" s="0" t="s">
         <v>15</v>
@@ -48804,19 +48808,19 @@
         <v>33001453</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D85" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F85" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E85" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="F85" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G85" s="0" t="s">
         <v>15</v>
@@ -48833,19 +48837,19 @@
         <v>33001553</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D86" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="F86" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E86" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="F86" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G86" s="0" t="s">
         <v>15</v>
@@ -48862,19 +48866,19 @@
         <v>33001635</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G87" s="0" t="s">
         <v>15</v>
@@ -48891,19 +48895,19 @@
         <v>33001695</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G88" s="0" t="s">
         <v>15</v>
@@ -48920,19 +48924,19 @@
         <v>33001735</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G89" s="0" t="s">
         <v>15</v>
@@ -48949,19 +48953,19 @@
         <v>33001835</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G90" s="0" t="s">
         <v>15</v>
@@ -48978,19 +48982,19 @@
         <v>33001953</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D91" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="F91" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E91" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="F91" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G91" s="0" t="s">
         <v>15</v>
@@ -49007,19 +49011,19 @@
         <v>33002053</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D92" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="F92" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="F92" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G92" s="0" t="s">
         <v>15</v>
@@ -49036,19 +49040,19 @@
         <v>33002135</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G93" s="0" t="s">
         <v>15</v>
@@ -49065,19 +49069,19 @@
         <v>33002195</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G94" s="0" t="s">
         <v>15</v>
@@ -49094,19 +49098,19 @@
         <v>33002235</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G95" s="0" t="s">
         <v>15</v>
@@ -49123,19 +49127,19 @@
         <v>33002295</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G96" s="0" t="s">
         <v>15</v>
@@ -49152,19 +49156,19 @@
         <v>33002353</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D97" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="F97" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="E97" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="F97" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="G97" s="0" t="s">
         <v>15</v>
@@ -49181,22 +49185,22 @@
         <v>33002499</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H98" s="0" t="s">
         <v>15</v>
@@ -49210,19 +49214,19 @@
         <v>33002535</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G99" s="0" t="s">
         <v>15</v>
@@ -49239,19 +49243,19 @@
         <v>33002635</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G100" s="0" t="s">
         <v>15</v>
@@ -49294,16 +49298,16 @@
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="1" s="6">
       <c r="A1" s="6" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -49314,10 +49318,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
@@ -49328,10 +49332,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
@@ -49342,10 +49346,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
@@ -49356,10 +49360,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
@@ -49370,10 +49374,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
@@ -49384,10 +49388,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
@@ -49398,10 +49402,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
@@ -49412,10 +49416,10 @@
         <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
@@ -49426,10 +49430,10 @@
         <v>36</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
@@ -49440,10 +49444,10 @@
         <v>37</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
@@ -49454,10 +49458,10 @@
         <v>62</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
@@ -49468,10 +49472,10 @@
         <v>63</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
@@ -49482,10 +49486,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
@@ -49496,10 +49500,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
@@ -49510,10 +49514,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
@@ -49524,10 +49528,10 @@
         <v>540</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
@@ -49538,10 +49542,10 @@
         <v>550</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
@@ -49552,10 +49556,10 @@
         <v>560</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
@@ -49566,10 +49570,10 @@
         <v>570</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
@@ -49580,10 +49584,10 @@
         <v>580</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
@@ -49594,10 +49598,10 @@
         <v>590</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
@@ -49608,10 +49612,10 @@
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
@@ -49622,10 +49626,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
@@ -49636,10 +49640,10 @@
         <v>3</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
@@ -49650,10 +49654,10 @@
         <v>30</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
@@ -49664,10 +49668,10 @@
         <v>920</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
@@ -49678,10 +49682,10 @@
         <v>930</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
@@ -49692,10 +49696,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
@@ -49706,10 +49710,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
@@ -49720,10 +49724,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
@@ -49734,10 +49738,10 @@
         <v>4</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
@@ -49748,10 +49752,10 @@
         <v>5</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
@@ -49762,10 +49766,10 @@
         <v>9</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
@@ -49776,10 +49780,10 @@
         <v>10</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
@@ -49790,10 +49794,10 @@
         <v>11</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
@@ -49804,10 +49808,10 @@
         <v>62</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
@@ -49818,10 +49822,10 @@
         <v>68</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
@@ -49832,10 +49836,10 @@
         <v>71</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
@@ -49846,10 +49850,10 @@
         <v>72</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
@@ -49860,10 +49864,10 @@
         <v>88</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
@@ -49874,10 +49878,10 @@
         <v>90</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>